<commit_message>
Les onglets fonctionnent correctement
</commit_message>
<xml_diff>
--- a/Temps de travail.xlsx
+++ b/Temps de travail.xlsx
@@ -1,25 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Users\amade\Documents\Gits\Lautrerive\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651A9983-974A-4C1A-8E18-C477E406D401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Jour</t>
+  </si>
+  <si>
+    <t>Heure début</t>
+  </si>
+  <si>
+    <t>Heure fin</t>
+  </si>
+  <si>
+    <t>Temps</t>
+  </si>
+  <si>
+    <t>Temps total</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="h&quot; h &quot;mm;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +87,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +370,327 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>44409</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="E2" s="2">
+        <f>D2-C2</f>
+        <v>4.7916666666666718E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>44410</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E42" si="0">D3-C3</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>44410</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.57916666666666672</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>5.8333333333333348E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>44410</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.6430555555555556</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>9.3055555555555558E-2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="2">
+        <f>SUM(E$2:E$1048576)</f>
+        <v>0.28263888888888894</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Suivi du temps de travail.
</commit_message>
<xml_diff>
--- a/Temps de travail.xlsx
+++ b/Temps de travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Users\amade\Documents\Gits\Lautrerive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651A9983-974A-4C1A-8E18-C477E406D401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589E70D8-8519-43DA-8F09-335EDE5214EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="h&quot; h &quot;mm;@"/>
+    <numFmt numFmtId="164" formatCode="h&quot; h &quot;mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -90,7 +90,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,7 +374,7 @@
   <dimension ref="B1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,14 +463,22 @@
       </c>
       <c r="K5" s="2">
         <f>SUM(E$2:E$1048576)</f>
-        <v>0.28263888888888894</v>
+        <v>0.41388888888888892</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
+      <c r="B6" s="1">
+        <v>44411</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.85</v>
+      </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.13124999999999998</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>